<commit_message>
Edits to counts for species list
CC
</commit_message>
<xml_diff>
--- a/Planning/Greenhouse and Raised Beds Map.xlsx
+++ b/Planning/Greenhouse and Raised Beds Map.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="212">
   <si>
     <t>SAMRAC08_GR</t>
   </si>
@@ -747,19 +747,13 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="146">
     <border>
@@ -2581,8 +2575,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="553">
+  <cellStyleXfs count="557">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3259,12 +3257,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3518,6 +3510,93 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="140" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3530,94 +3609,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="141" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3656,24 +3666,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="144" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3776,8 +3768,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="553">
+  <cellStyles count="557">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4054,6 +4052,8 @@
     <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4330,6 +4330,8 @@
     <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4665,24 +4667,24 @@
   <dimension ref="C1:BC21"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:AF1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="3:55" ht="35" customHeight="1">
-      <c r="W1" s="131" t="s">
+      <c r="W1" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="132"/>
-      <c r="Y1" s="132"/>
-      <c r="Z1" s="132"/>
-      <c r="AA1" s="132"/>
-      <c r="AB1" s="132"/>
-      <c r="AC1" s="132"/>
-      <c r="AD1" s="132"/>
-      <c r="AE1" s="132"/>
-      <c r="AF1" s="132"/>
+      <c r="X1" s="159"/>
+      <c r="Y1" s="159"/>
+      <c r="Z1" s="159"/>
+      <c r="AA1" s="159"/>
+      <c r="AB1" s="159"/>
+      <c r="AC1" s="159"/>
+      <c r="AD1" s="159"/>
+      <c r="AE1" s="159"/>
+      <c r="AF1" s="159"/>
     </row>
     <row r="2" spans="3:55" ht="35" customHeight="1" thickBot="1"/>
     <row r="3" spans="3:55" ht="35" customHeight="1" thickTop="1">
@@ -5764,183 +5766,194 @@
       <c r="AX14" s="25"/>
       <c r="AY14" s="1"/>
       <c r="AZ14" s="35"/>
-      <c r="BA14" s="133" t="s">
+      <c r="BA14" s="127" t="s">
         <v>45</v>
       </c>
-      <c r="BB14" s="134"/>
-      <c r="BC14" s="135"/>
+      <c r="BB14" s="128"/>
+      <c r="BC14" s="129"/>
     </row>
     <row r="15" spans="3:55" ht="35" customHeight="1" thickTop="1">
-      <c r="C15" s="157" t="s">
+      <c r="C15" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="157" t="s">
+      <c r="D15" s="152"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="160"/>
-      <c r="M15" s="161" t="s">
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="153"/>
+      <c r="M15" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="158"/>
-      <c r="O15" s="158"/>
-      <c r="P15" s="158"/>
-      <c r="Q15" s="160"/>
-      <c r="R15" s="157" t="s">
+      <c r="N15" s="152"/>
+      <c r="O15" s="152"/>
+      <c r="P15" s="152"/>
+      <c r="Q15" s="153"/>
+      <c r="R15" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="S15" s="158"/>
-      <c r="T15" s="158"/>
-      <c r="U15" s="158"/>
-      <c r="V15" s="160"/>
-      <c r="W15" s="161" t="s">
+      <c r="S15" s="152"/>
+      <c r="T15" s="152"/>
+      <c r="U15" s="152"/>
+      <c r="V15" s="153"/>
+      <c r="W15" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="X15" s="158"/>
-      <c r="Y15" s="158"/>
-      <c r="Z15" s="158"/>
-      <c r="AA15" s="160"/>
-      <c r="AB15" s="142" t="s">
+      <c r="X15" s="152"/>
+      <c r="Y15" s="152"/>
+      <c r="Z15" s="152"/>
+      <c r="AA15" s="153"/>
+      <c r="AB15" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="AC15" s="143"/>
-      <c r="AD15" s="143"/>
-      <c r="AE15" s="143"/>
-      <c r="AF15" s="144"/>
-      <c r="AG15" s="147" t="s">
+      <c r="AC15" s="137"/>
+      <c r="AD15" s="137"/>
+      <c r="AE15" s="137"/>
+      <c r="AF15" s="138"/>
+      <c r="AG15" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="AH15" s="143"/>
-      <c r="AI15" s="143"/>
-      <c r="AJ15" s="143"/>
-      <c r="AK15" s="144"/>
-      <c r="AL15" s="147" t="s">
+      <c r="AH15" s="137"/>
+      <c r="AI15" s="137"/>
+      <c r="AJ15" s="137"/>
+      <c r="AK15" s="138"/>
+      <c r="AL15" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="AM15" s="143"/>
-      <c r="AN15" s="143"/>
-      <c r="AO15" s="143"/>
-      <c r="AP15" s="162"/>
-      <c r="AQ15" s="152" t="s">
+      <c r="AM15" s="137"/>
+      <c r="AN15" s="137"/>
+      <c r="AO15" s="137"/>
+      <c r="AP15" s="155"/>
+      <c r="AQ15" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="AR15" s="153"/>
-      <c r="AS15" s="153"/>
-      <c r="AT15" s="153"/>
-      <c r="AU15" s="154"/>
-      <c r="AV15" s="155" t="s">
+      <c r="AR15" s="147"/>
+      <c r="AS15" s="147"/>
+      <c r="AT15" s="147"/>
+      <c r="AU15" s="148"/>
+      <c r="AV15" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="AW15" s="153"/>
-      <c r="AX15" s="153"/>
-      <c r="AY15" s="153"/>
-      <c r="AZ15" s="156"/>
-      <c r="BA15" s="136"/>
-      <c r="BB15" s="137"/>
-      <c r="BC15" s="138"/>
+      <c r="AW15" s="147"/>
+      <c r="AX15" s="147"/>
+      <c r="AY15" s="147"/>
+      <c r="AZ15" s="150"/>
+      <c r="BA15" s="130"/>
+      <c r="BB15" s="131"/>
+      <c r="BC15" s="132"/>
     </row>
     <row r="16" spans="3:55" ht="35" customHeight="1" thickBot="1">
-      <c r="C16" s="145" t="s">
+      <c r="C16" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="146"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="146"/>
-      <c r="G16" s="151"/>
-      <c r="H16" s="145" t="s">
+      <c r="D16" s="140"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="145"/>
+      <c r="H16" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="146"/>
-      <c r="J16" s="146"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="146"/>
-      <c r="M16" s="146"/>
-      <c r="N16" s="146"/>
-      <c r="O16" s="146"/>
-      <c r="P16" s="146"/>
-      <c r="Q16" s="146"/>
-      <c r="R16" s="145" t="s">
+      <c r="I16" s="140"/>
+      <c r="J16" s="140"/>
+      <c r="K16" s="140"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="140"/>
+      <c r="P16" s="140"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="139" t="s">
         <v>42</v>
       </c>
-      <c r="S16" s="146"/>
-      <c r="T16" s="146"/>
-      <c r="U16" s="146"/>
-      <c r="V16" s="146"/>
-      <c r="W16" s="146"/>
-      <c r="X16" s="146"/>
-      <c r="Y16" s="146"/>
-      <c r="Z16" s="146"/>
-      <c r="AA16" s="146"/>
-      <c r="AB16" s="148" t="s">
+      <c r="S16" s="140"/>
+      <c r="T16" s="140"/>
+      <c r="U16" s="140"/>
+      <c r="V16" s="140"/>
+      <c r="W16" s="140"/>
+      <c r="X16" s="140"/>
+      <c r="Y16" s="140"/>
+      <c r="Z16" s="140"/>
+      <c r="AA16" s="140"/>
+      <c r="AB16" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="AC16" s="149"/>
-      <c r="AD16" s="149"/>
-      <c r="AE16" s="149"/>
-      <c r="AF16" s="149"/>
-      <c r="AG16" s="149"/>
-      <c r="AH16" s="149"/>
-      <c r="AI16" s="149"/>
-      <c r="AJ16" s="149"/>
-      <c r="AK16" s="149"/>
-      <c r="AL16" s="149"/>
-      <c r="AM16" s="149"/>
-      <c r="AN16" s="149"/>
-      <c r="AO16" s="149"/>
-      <c r="AP16" s="150"/>
-      <c r="AQ16" s="145" t="s">
+      <c r="AC16" s="143"/>
+      <c r="AD16" s="143"/>
+      <c r="AE16" s="143"/>
+      <c r="AF16" s="143"/>
+      <c r="AG16" s="143"/>
+      <c r="AH16" s="143"/>
+      <c r="AI16" s="143"/>
+      <c r="AJ16" s="143"/>
+      <c r="AK16" s="143"/>
+      <c r="AL16" s="143"/>
+      <c r="AM16" s="143"/>
+      <c r="AN16" s="143"/>
+      <c r="AO16" s="143"/>
+      <c r="AP16" s="144"/>
+      <c r="AQ16" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="AR16" s="146"/>
-      <c r="AS16" s="146"/>
-      <c r="AT16" s="146"/>
-      <c r="AU16" s="146"/>
-      <c r="AV16" s="146"/>
-      <c r="AW16" s="146"/>
-      <c r="AX16" s="146"/>
-      <c r="AY16" s="146"/>
-      <c r="AZ16" s="151"/>
-      <c r="BA16" s="139"/>
-      <c r="BB16" s="140"/>
-      <c r="BC16" s="141"/>
-    </row>
-    <row r="17" spans="3:7" ht="35" customHeight="1" thickTop="1"/>
-    <row r="18" spans="3:7" ht="35" customHeight="1">
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
+      <c r="AR16" s="140"/>
+      <c r="AS16" s="140"/>
+      <c r="AT16" s="140"/>
+      <c r="AU16" s="140"/>
+      <c r="AV16" s="140"/>
+      <c r="AW16" s="140"/>
+      <c r="AX16" s="140"/>
+      <c r="AY16" s="140"/>
+      <c r="AZ16" s="145"/>
+      <c r="BA16" s="133"/>
+      <c r="BB16" s="134"/>
+      <c r="BC16" s="135"/>
+    </row>
+    <row r="17" spans="3:11" ht="35" customHeight="1" thickTop="1"/>
+    <row r="18" spans="3:11" ht="35" customHeight="1">
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="3:7" ht="35" customHeight="1">
+    <row r="19" spans="3:11" ht="35" customHeight="1">
       <c r="C19" s="11"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="156"/>
+      <c r="F19" s="156"/>
       <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="3:7" ht="35" customHeight="1">
+      <c r="K19">
+        <f>COUNTIF(C3:AZ14,"*")</f>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" ht="35" customHeight="1">
       <c r="C20" s="11"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="3:7" ht="35" customHeight="1">
+    <row r="21" spans="3:11" ht="35" customHeight="1">
       <c r="C21" s="11"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="129"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="W1:AF1"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C15:G15"/>
     <mergeCell ref="BA14:BC16"/>
     <mergeCell ref="AB15:AF15"/>
     <mergeCell ref="H16:Q16"/>
@@ -5955,13 +5968,6 @@
     <mergeCell ref="R15:V15"/>
     <mergeCell ref="W15:AA15"/>
     <mergeCell ref="AL15:AP15"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="W1:AF1"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C15:G15"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions verticalCentered="1"/>
@@ -6626,72 +6632,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:BG34"/>
+  <dimension ref="C1:BG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="AI9" sqref="AI9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="5:59" ht="35" customHeight="1">
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="131" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="158" t="s">
         <v>211</v>
       </c>
-      <c r="Z1" s="131"/>
-      <c r="AA1" s="131"/>
-      <c r="AB1" s="131"/>
-      <c r="AC1" s="131"/>
-      <c r="AD1" s="131"/>
-      <c r="AE1" s="131"/>
-      <c r="AF1" s="131"/>
-      <c r="AG1" s="131"/>
-      <c r="AH1" s="131"/>
-      <c r="AI1" s="131"/>
-      <c r="AJ1" s="131"/>
-      <c r="AK1" s="131"/>
-      <c r="AL1" s="131"/>
-      <c r="AM1" s="131"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="58"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="58"/>
-      <c r="AV1" s="58"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="58"/>
-      <c r="AY1" s="58"/>
-      <c r="AZ1" s="58"/>
-      <c r="BA1" s="58"/>
-      <c r="BB1" s="58"/>
-      <c r="BC1" s="58"/>
-      <c r="BD1" s="58"/>
-      <c r="BE1" s="58"/>
-      <c r="BF1" s="58"/>
-      <c r="BG1" s="58"/>
+      <c r="Z1" s="158"/>
+      <c r="AA1" s="158"/>
+      <c r="AB1" s="158"/>
+      <c r="AC1" s="158"/>
+      <c r="AD1" s="158"/>
+      <c r="AE1" s="158"/>
+      <c r="AF1" s="158"/>
+      <c r="AG1" s="158"/>
+      <c r="AH1" s="158"/>
+      <c r="AI1" s="158"/>
+      <c r="AJ1" s="158"/>
+      <c r="AK1" s="158"/>
+      <c r="AL1" s="158"/>
+      <c r="AM1" s="158"/>
+      <c r="AN1" s="56"/>
+      <c r="AO1" s="56"/>
+      <c r="AP1" s="56"/>
+      <c r="AQ1" s="56"/>
+      <c r="AR1" s="56"/>
+      <c r="AS1" s="56"/>
+      <c r="AT1" s="56"/>
+      <c r="AU1" s="56"/>
+      <c r="AV1" s="56"/>
+      <c r="AW1" s="56"/>
+      <c r="AX1" s="56"/>
+      <c r="AY1" s="56"/>
+      <c r="AZ1" s="56"/>
+      <c r="BA1" s="56"/>
+      <c r="BB1" s="56"/>
+      <c r="BC1" s="56"/>
+      <c r="BD1" s="56"/>
+      <c r="BE1" s="56"/>
+      <c r="BF1" s="56"/>
+      <c r="BG1" s="56"/>
     </row>
     <row r="2" spans="5:59" ht="35" customHeight="1" thickBot="1"/>
     <row r="3" spans="5:59" ht="35" customHeight="1" thickTop="1">
@@ -6745,7 +6751,7 @@
       <c r="AZ3" s="14"/>
       <c r="BA3" s="5"/>
       <c r="BB3" s="15"/>
-      <c r="BC3" s="44"/>
+      <c r="BC3" s="42"/>
       <c r="BD3" s="5"/>
       <c r="BE3" s="14"/>
       <c r="BF3" s="5"/>
@@ -6817,7 +6823,7 @@
       <c r="AY4" s="12"/>
       <c r="AZ4" s="12"/>
       <c r="BA4" s="12"/>
-      <c r="BB4" s="48"/>
+      <c r="BB4" s="46"/>
       <c r="BC4" s="3"/>
       <c r="BD4" s="12"/>
       <c r="BE4" s="12"/>
@@ -6889,7 +6895,7 @@
       <c r="AZ5" s="17"/>
       <c r="BA5" s="8"/>
       <c r="BB5" s="16"/>
-      <c r="BC5" s="45"/>
+      <c r="BC5" s="43"/>
       <c r="BD5" s="8"/>
       <c r="BE5" s="17"/>
       <c r="BF5" s="8"/>
@@ -6960,7 +6966,7 @@
       <c r="AZ6" s="20"/>
       <c r="BA6" s="9"/>
       <c r="BB6" s="21"/>
-      <c r="BC6" s="46"/>
+      <c r="BC6" s="44"/>
       <c r="BD6" s="9"/>
       <c r="BE6" s="20"/>
       <c r="BF6" s="9"/>
@@ -7030,7 +7036,7 @@
       <c r="AY7" s="12"/>
       <c r="AZ7" s="12"/>
       <c r="BA7" s="12"/>
-      <c r="BB7" s="49"/>
+      <c r="BB7" s="47"/>
       <c r="BC7" s="3"/>
       <c r="BD7" s="12"/>
       <c r="BE7" s="12"/>
@@ -7100,7 +7106,7 @@
       <c r="AZ8" s="17"/>
       <c r="BA8" s="8"/>
       <c r="BB8" s="16"/>
-      <c r="BC8" s="45"/>
+      <c r="BC8" s="43"/>
       <c r="BD8" s="8"/>
       <c r="BE8" s="17"/>
       <c r="BF8" s="8"/>
@@ -7175,7 +7181,7 @@
       <c r="AZ9" s="20"/>
       <c r="BA9" s="9"/>
       <c r="BB9" s="21"/>
-      <c r="BC9" s="46"/>
+      <c r="BC9" s="44"/>
       <c r="BD9" s="9"/>
       <c r="BE9" s="20"/>
       <c r="BF9" s="9"/>
@@ -7251,7 +7257,7 @@
       <c r="AY10" s="12"/>
       <c r="AZ10" s="12"/>
       <c r="BA10" s="12"/>
-      <c r="BB10" s="48"/>
+      <c r="BB10" s="46"/>
       <c r="BC10" s="3"/>
       <c r="BD10" s="12"/>
       <c r="BE10" s="12"/>
@@ -7327,7 +7333,7 @@
       <c r="AZ11" s="17"/>
       <c r="BA11" s="8"/>
       <c r="BB11" s="16"/>
-      <c r="BC11" s="45"/>
+      <c r="BC11" s="43"/>
       <c r="BD11" s="8"/>
       <c r="BE11" s="17"/>
       <c r="BF11" s="8"/>
@@ -7404,7 +7410,7 @@
       <c r="AZ12" s="20"/>
       <c r="BA12" s="9"/>
       <c r="BB12" s="21"/>
-      <c r="BC12" s="46"/>
+      <c r="BC12" s="44"/>
       <c r="BD12" s="9"/>
       <c r="BE12" s="20"/>
       <c r="BF12" s="9"/>
@@ -7480,7 +7486,7 @@
       <c r="AY13" s="12"/>
       <c r="AZ13" s="12"/>
       <c r="BA13" s="12"/>
-      <c r="BB13" s="49"/>
+      <c r="BB13" s="47"/>
       <c r="BC13" s="3"/>
       <c r="BD13" s="12"/>
       <c r="BE13" s="12"/>
@@ -7558,7 +7564,7 @@
       <c r="AZ14" s="17"/>
       <c r="BA14" s="41"/>
       <c r="BB14" s="16"/>
-      <c r="BC14" s="45"/>
+      <c r="BC14" s="43"/>
       <c r="BD14" s="41"/>
       <c r="BE14" s="17"/>
       <c r="BF14" s="41"/>
@@ -7645,7 +7651,7 @@
       <c r="AZ15" s="27"/>
       <c r="BA15" s="3"/>
       <c r="BB15" s="38"/>
-      <c r="BC15" s="47"/>
+      <c r="BC15" s="45"/>
       <c r="BD15" s="3"/>
       <c r="BE15" s="27"/>
       <c r="BF15" s="3"/>
@@ -7739,7 +7745,7 @@
       <c r="AY16" s="12"/>
       <c r="AZ16" s="12"/>
       <c r="BA16" s="12"/>
-      <c r="BB16" s="48"/>
+      <c r="BB16" s="46"/>
       <c r="BC16" s="3"/>
       <c r="BD16" s="12"/>
       <c r="BE16" s="12"/>
@@ -7833,7 +7839,7 @@
       <c r="AZ17" s="17"/>
       <c r="BA17" s="8"/>
       <c r="BB17" s="16"/>
-      <c r="BC17" s="45"/>
+      <c r="BC17" s="43"/>
       <c r="BD17" s="8"/>
       <c r="BE17" s="17"/>
       <c r="BF17" s="8"/>
@@ -7940,7 +7946,7 @@
       <c r="BB18" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="BC18" s="46"/>
+      <c r="BC18" s="44"/>
       <c r="BD18" s="9"/>
       <c r="BE18" s="20"/>
       <c r="BF18" s="9"/>
@@ -8044,7 +8050,7 @@
       <c r="BA19" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="BB19" s="49" t="s">
+      <c r="BB19" s="47" t="s">
         <v>149</v>
       </c>
       <c r="BC19" s="3" t="s">
@@ -8164,7 +8170,7 @@
       <c r="BB20" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="BC20" s="46" t="s">
+      <c r="BC20" s="44" t="s">
         <v>166</v>
       </c>
       <c r="BD20" s="19" t="s">
@@ -8237,13 +8243,15 @@
       <c r="AJ21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AK21" s="43" t="s">
+      <c r="AK21" s="213" t="s">
         <v>96</v>
       </c>
       <c r="AL21" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AM21" s="21"/>
+      <c r="AM21" s="213" t="s">
+        <v>96</v>
+      </c>
       <c r="AN21" s="19" t="s">
         <v>66</v>
       </c>
@@ -8285,7 +8293,7 @@
       <c r="BB21" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="BC21" s="46" t="s">
+      <c r="BC21" s="44" t="s">
         <v>166</v>
       </c>
       <c r="BD21" s="19" t="s">
@@ -8401,7 +8409,7 @@
       <c r="BA22" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="BB22" s="48" t="s">
+      <c r="BB22" s="46" t="s">
         <v>148</v>
       </c>
       <c r="BC22" s="3" t="s">
@@ -8523,7 +8531,7 @@
       <c r="BB23" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="BC23" s="45" t="s">
+      <c r="BC23" s="43" t="s">
         <v>144</v>
       </c>
       <c r="BD23" s="22" t="s">
@@ -8575,13 +8583,21 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="9"/>
       <c r="AC24" s="21"/>
-      <c r="AD24" s="42" t="s">
+      <c r="AD24" s="214" t="s">
         <v>78</v>
       </c>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="20"/>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="21"/>
+      <c r="AE24" s="214" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF24" s="214" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG24" s="214" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH24" s="214" t="s">
+        <v>78</v>
+      </c>
       <c r="AI24" s="19" t="s">
         <v>97</v>
       </c>
@@ -8634,7 +8650,7 @@
         <v>163</v>
       </c>
       <c r="BB24" s="21"/>
-      <c r="BC24" s="46" t="s">
+      <c r="BC24" s="44" t="s">
         <v>139</v>
       </c>
       <c r="BD24" s="9" t="s">
@@ -8752,7 +8768,7 @@
       <c r="BA25" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="BB25" s="49" t="s">
+      <c r="BB25" s="47" t="s">
         <v>163</v>
       </c>
       <c r="BC25" s="3" t="s">
@@ -8892,7 +8908,7 @@
       <c r="BB26" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="BC26" s="45" t="s">
+      <c r="BC26" s="43" t="s">
         <v>162</v>
       </c>
       <c r="BD26" s="41" t="s">
@@ -9027,7 +9043,7 @@
       </c>
       <c r="BA27" s="3"/>
       <c r="BB27" s="38"/>
-      <c r="BC27" s="47" t="s">
+      <c r="BC27" s="45" t="s">
         <v>160</v>
       </c>
       <c r="BD27" s="3" t="s">
@@ -9173,7 +9189,7 @@
       <c r="AY28" s="12"/>
       <c r="AZ28" s="12"/>
       <c r="BA28" s="12"/>
-      <c r="BB28" s="48"/>
+      <c r="BB28" s="46"/>
       <c r="BC28" s="3" t="s">
         <v>161</v>
       </c>
@@ -9315,7 +9331,7 @@
       <c r="AZ29" s="17"/>
       <c r="BA29" s="8"/>
       <c r="BB29" s="16"/>
-      <c r="BC29" s="45" t="s">
+      <c r="BC29" s="43" t="s">
         <v>160</v>
       </c>
       <c r="BD29" s="22" t="s">
@@ -9458,7 +9474,7 @@
         <v>16</v>
       </c>
       <c r="BB30" s="21"/>
-      <c r="BC30" s="46" t="s">
+      <c r="BC30" s="44" t="s">
         <v>160</v>
       </c>
       <c r="BD30" s="9" t="s">
@@ -9594,7 +9610,7 @@
         <v>16</v>
       </c>
       <c r="BA31" s="12"/>
-      <c r="BB31" s="49"/>
+      <c r="BB31" s="47"/>
       <c r="BC31" s="3" t="s">
         <v>159</v>
       </c>
@@ -9608,49 +9624,49 @@
       <c r="BG31" s="7"/>
     </row>
     <row r="32" spans="3:59" ht="35" customHeight="1" thickBot="1">
-      <c r="C32" s="175" t="s">
+      <c r="C32" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="176"/>
-      <c r="E32" s="125" t="s">
+      <c r="D32" s="162"/>
+      <c r="E32" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="126" t="s">
+      <c r="F32" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="96" t="s">
+      <c r="G32" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="H32" s="126" t="s">
+      <c r="H32" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="I32" s="98"/>
-      <c r="J32" s="127" t="s">
+      <c r="I32" s="96"/>
+      <c r="J32" s="125" t="s">
         <v>58</v>
       </c>
-      <c r="K32" s="126" t="s">
+      <c r="K32" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="L32" s="96" t="s">
+      <c r="L32" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="M32" s="126" t="s">
+      <c r="M32" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="N32" s="98" t="s">
+      <c r="N32" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="O32" s="127" t="s">
+      <c r="O32" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="P32" s="126" t="s">
+      <c r="P32" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="Q32" s="96" t="s">
+      <c r="Q32" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="R32" s="126"/>
-      <c r="S32" s="98"/>
+      <c r="R32" s="124"/>
+      <c r="S32" s="96"/>
       <c r="T32" s="24" t="s">
         <v>74</v>
       </c>
@@ -9733,182 +9749,183 @@
       <c r="AU32" s="25"/>
       <c r="AV32" s="36"/>
       <c r="AW32" s="26"/>
-      <c r="AX32" s="127" t="s">
+      <c r="AX32" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="AY32" s="126" t="s">
+      <c r="AY32" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="AZ32" s="96"/>
-      <c r="BA32" s="126"/>
-      <c r="BB32" s="98"/>
-      <c r="BC32" s="125" t="s">
+      <c r="AZ32" s="94"/>
+      <c r="BA32" s="124"/>
+      <c r="BB32" s="96"/>
+      <c r="BC32" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="BD32" s="126" t="s">
+      <c r="BD32" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="BE32" s="96" t="s">
+      <c r="BE32" s="94" t="s">
         <v>159</v>
       </c>
-      <c r="BF32" s="126"/>
-      <c r="BG32" s="128"/>
+      <c r="BF32" s="124"/>
+      <c r="BG32" s="126"/>
     </row>
     <row r="33" spans="3:59" ht="35" customHeight="1" thickTop="1">
-      <c r="C33" s="177"/>
-      <c r="D33" s="178"/>
-      <c r="E33" s="166" t="s">
+      <c r="C33" s="163"/>
+      <c r="D33" s="164"/>
+      <c r="E33" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="167"/>
-      <c r="G33" s="167"/>
-      <c r="H33" s="167"/>
-      <c r="I33" s="168"/>
-      <c r="J33" s="169" t="s">
+      <c r="F33" s="171"/>
+      <c r="G33" s="171"/>
+      <c r="H33" s="171"/>
+      <c r="I33" s="172"/>
+      <c r="J33" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="K33" s="167"/>
-      <c r="L33" s="167"/>
-      <c r="M33" s="167"/>
-      <c r="N33" s="168"/>
-      <c r="O33" s="169" t="s">
+      <c r="K33" s="171"/>
+      <c r="L33" s="171"/>
+      <c r="M33" s="171"/>
+      <c r="N33" s="172"/>
+      <c r="O33" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="P33" s="167"/>
-      <c r="Q33" s="167"/>
-      <c r="R33" s="167"/>
-      <c r="S33" s="170"/>
-      <c r="T33" s="174" t="s">
+      <c r="P33" s="171"/>
+      <c r="Q33" s="171"/>
+      <c r="R33" s="171"/>
+      <c r="S33" s="174"/>
+      <c r="T33" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="U33" s="158"/>
-      <c r="V33" s="158"/>
-      <c r="W33" s="158"/>
-      <c r="X33" s="160"/>
-      <c r="Y33" s="161" t="s">
+      <c r="U33" s="152"/>
+      <c r="V33" s="152"/>
+      <c r="W33" s="152"/>
+      <c r="X33" s="153"/>
+      <c r="Y33" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="Z33" s="158"/>
-      <c r="AA33" s="158"/>
-      <c r="AB33" s="158"/>
-      <c r="AC33" s="160"/>
-      <c r="AD33" s="161" t="s">
+      <c r="Z33" s="152"/>
+      <c r="AA33" s="152"/>
+      <c r="AB33" s="152"/>
+      <c r="AC33" s="153"/>
+      <c r="AD33" s="154" t="s">
         <v>37</v>
       </c>
-      <c r="AE33" s="158"/>
-      <c r="AF33" s="158"/>
-      <c r="AG33" s="158"/>
-      <c r="AH33" s="171"/>
-      <c r="AI33" s="174" t="s">
+      <c r="AE33" s="152"/>
+      <c r="AF33" s="152"/>
+      <c r="AG33" s="152"/>
+      <c r="AH33" s="175"/>
+      <c r="AI33" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="AJ33" s="158"/>
-      <c r="AK33" s="158"/>
-      <c r="AL33" s="158"/>
-      <c r="AM33" s="160"/>
-      <c r="AN33" s="161" t="s">
+      <c r="AJ33" s="152"/>
+      <c r="AK33" s="152"/>
+      <c r="AL33" s="152"/>
+      <c r="AM33" s="153"/>
+      <c r="AN33" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="AO33" s="158"/>
-      <c r="AP33" s="158"/>
-      <c r="AQ33" s="158"/>
-      <c r="AR33" s="160"/>
-      <c r="AS33" s="161" t="s">
+      <c r="AO33" s="152"/>
+      <c r="AP33" s="152"/>
+      <c r="AQ33" s="152"/>
+      <c r="AR33" s="153"/>
+      <c r="AS33" s="154" t="s">
         <v>37</v>
       </c>
-      <c r="AT33" s="158"/>
-      <c r="AU33" s="158"/>
-      <c r="AV33" s="158"/>
-      <c r="AW33" s="171"/>
-      <c r="AX33" s="166" t="s">
+      <c r="AT33" s="152"/>
+      <c r="AU33" s="152"/>
+      <c r="AV33" s="152"/>
+      <c r="AW33" s="175"/>
+      <c r="AX33" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="AY33" s="167"/>
-      <c r="AZ33" s="167"/>
-      <c r="BA33" s="167"/>
-      <c r="BB33" s="168"/>
-      <c r="BC33" s="169" t="s">
+      <c r="AY33" s="171"/>
+      <c r="AZ33" s="171"/>
+      <c r="BA33" s="171"/>
+      <c r="BB33" s="172"/>
+      <c r="BC33" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="BD33" s="167"/>
-      <c r="BE33" s="167"/>
-      <c r="BF33" s="167"/>
-      <c r="BG33" s="170"/>
+      <c r="BD33" s="171"/>
+      <c r="BE33" s="171"/>
+      <c r="BF33" s="171"/>
+      <c r="BG33" s="174"/>
     </row>
     <row r="34" spans="3:59" ht="35" customHeight="1" thickBot="1">
-      <c r="C34" s="179"/>
-      <c r="D34" s="180"/>
-      <c r="E34" s="163" t="s">
+      <c r="C34" s="165"/>
+      <c r="D34" s="166"/>
+      <c r="E34" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="164"/>
-      <c r="G34" s="164"/>
-      <c r="H34" s="164"/>
-      <c r="I34" s="164"/>
-      <c r="J34" s="164"/>
-      <c r="K34" s="164"/>
-      <c r="L34" s="164"/>
-      <c r="M34" s="164"/>
-      <c r="N34" s="164"/>
-      <c r="O34" s="164"/>
-      <c r="P34" s="164"/>
-      <c r="Q34" s="164"/>
-      <c r="R34" s="164"/>
-      <c r="S34" s="165"/>
-      <c r="T34" s="163" t="s">
+      <c r="F34" s="168"/>
+      <c r="G34" s="168"/>
+      <c r="H34" s="168"/>
+      <c r="I34" s="168"/>
+      <c r="J34" s="168"/>
+      <c r="K34" s="168"/>
+      <c r="L34" s="168"/>
+      <c r="M34" s="168"/>
+      <c r="N34" s="168"/>
+      <c r="O34" s="168"/>
+      <c r="P34" s="168"/>
+      <c r="Q34" s="168"/>
+      <c r="R34" s="168"/>
+      <c r="S34" s="169"/>
+      <c r="T34" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="U34" s="172"/>
-      <c r="V34" s="172"/>
-      <c r="W34" s="172"/>
-      <c r="X34" s="172"/>
-      <c r="Y34" s="172"/>
-      <c r="Z34" s="172"/>
-      <c r="AA34" s="172"/>
-      <c r="AB34" s="172"/>
-      <c r="AC34" s="172"/>
-      <c r="AD34" s="172"/>
-      <c r="AE34" s="172"/>
-      <c r="AF34" s="172"/>
-      <c r="AG34" s="172"/>
-      <c r="AH34" s="173"/>
-      <c r="AI34" s="163" t="s">
+      <c r="U34" s="176"/>
+      <c r="V34" s="176"/>
+      <c r="W34" s="176"/>
+      <c r="X34" s="176"/>
+      <c r="Y34" s="176"/>
+      <c r="Z34" s="176"/>
+      <c r="AA34" s="176"/>
+      <c r="AB34" s="176"/>
+      <c r="AC34" s="176"/>
+      <c r="AD34" s="176"/>
+      <c r="AE34" s="176"/>
+      <c r="AF34" s="176"/>
+      <c r="AG34" s="176"/>
+      <c r="AH34" s="177"/>
+      <c r="AI34" s="167" t="s">
         <v>40</v>
       </c>
-      <c r="AJ34" s="172"/>
-      <c r="AK34" s="172"/>
-      <c r="AL34" s="172"/>
-      <c r="AM34" s="172"/>
-      <c r="AN34" s="172"/>
-      <c r="AO34" s="172"/>
-      <c r="AP34" s="172"/>
-      <c r="AQ34" s="172"/>
-      <c r="AR34" s="172"/>
-      <c r="AS34" s="172"/>
-      <c r="AT34" s="172"/>
-      <c r="AU34" s="172"/>
-      <c r="AV34" s="172"/>
-      <c r="AW34" s="173"/>
-      <c r="AX34" s="163" t="s">
+      <c r="AJ34" s="176"/>
+      <c r="AK34" s="176"/>
+      <c r="AL34" s="176"/>
+      <c r="AM34" s="176"/>
+      <c r="AN34" s="176"/>
+      <c r="AO34" s="176"/>
+      <c r="AP34" s="176"/>
+      <c r="AQ34" s="176"/>
+      <c r="AR34" s="176"/>
+      <c r="AS34" s="176"/>
+      <c r="AT34" s="176"/>
+      <c r="AU34" s="176"/>
+      <c r="AV34" s="176"/>
+      <c r="AW34" s="177"/>
+      <c r="AX34" s="167" t="s">
         <v>39</v>
       </c>
-      <c r="AY34" s="164"/>
-      <c r="AZ34" s="164"/>
-      <c r="BA34" s="164"/>
-      <c r="BB34" s="164"/>
-      <c r="BC34" s="164"/>
-      <c r="BD34" s="164"/>
-      <c r="BE34" s="164"/>
-      <c r="BF34" s="164"/>
-      <c r="BG34" s="165"/>
+      <c r="AY34" s="168"/>
+      <c r="AZ34" s="168"/>
+      <c r="BA34" s="168"/>
+      <c r="BB34" s="168"/>
+      <c r="BC34" s="168"/>
+      <c r="BD34" s="168"/>
+      <c r="BE34" s="168"/>
+      <c r="BF34" s="168"/>
+      <c r="BG34" s="169"/>
+    </row>
+    <row r="37" spans="3:59" ht="35" customHeight="1">
+      <c r="O37">
+        <f>COUNTIF(E3:BG32,"*")</f>
+        <v>678</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C32:D34"/>
-    <mergeCell ref="E34:S34"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:S33"/>
     <mergeCell ref="AX34:BG34"/>
     <mergeCell ref="AX33:BB33"/>
     <mergeCell ref="BC33:BG33"/>
@@ -9921,6 +9938,11 @@
     <mergeCell ref="AS33:AW33"/>
     <mergeCell ref="AI34:AW34"/>
     <mergeCell ref="T33:X33"/>
+    <mergeCell ref="C32:D34"/>
+    <mergeCell ref="E34:S34"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:S33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11520,374 +11542,390 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="C1" s="193" t="s">
+    <row r="1" spans="1:13">
+      <c r="C1" s="191" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="193"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
-      <c r="I2" s="193"/>
-      <c r="J2" s="193"/>
-      <c r="K2" s="193"/>
-    </row>
-    <row r="3" spans="1:11" ht="16" thickBot="1"/>
-    <row r="4" spans="1:11" ht="16" thickTop="1">
-      <c r="C4" s="50" t="s">
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+    </row>
+    <row r="3" spans="1:13" ht="16" thickBot="1"/>
+    <row r="4" spans="1:13" ht="16" thickTop="1">
+      <c r="C4" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="57" t="s">
         <v>168</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="64"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="184" t="s">
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="62"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="182" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="181" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182"/>
-      <c r="K5" s="183"/>
-    </row>
-    <row r="6" spans="1:11" ht="16" thickBot="1">
-      <c r="A6" s="185"/>
-      <c r="C6" s="54" t="s">
+      <c r="I5" s="180"/>
+      <c r="J5" s="180"/>
+      <c r="K5" s="181"/>
+    </row>
+    <row r="6" spans="1:13" ht="16" thickBot="1">
+      <c r="A6" s="183"/>
+      <c r="C6" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="65"/>
-    </row>
-    <row r="7" spans="1:11" ht="16" thickTop="1">
-      <c r="A7" s="185"/>
-    </row>
-    <row r="8" spans="1:11" ht="16" thickBot="1">
-      <c r="A8" s="185"/>
-    </row>
-    <row r="9" spans="1:11" ht="16" thickTop="1">
-      <c r="A9" s="185"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59" t="s">
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="63"/>
+    </row>
+    <row r="7" spans="1:13" ht="16" thickTop="1">
+      <c r="A7" s="183"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" thickBot="1">
+      <c r="A8" s="183"/>
+    </row>
+    <row r="9" spans="1:13" ht="16" thickTop="1">
+      <c r="A9" s="183"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="57" t="s">
         <v>173</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="K9" s="64" t="s">
+      <c r="K9" s="62" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="185"/>
-      <c r="C10" s="63" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="183"/>
+      <c r="C10" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60" t="s">
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="K10" s="66" t="s">
+      <c r="K10" s="64" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="16" thickBot="1">
-      <c r="A11" s="185"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61" t="s">
+      <c r="M10">
+        <f>COUNTIF(C14:K20,"*")</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" thickBot="1">
+      <c r="A11" s="183"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="G11" s="61" t="s">
+      <c r="G11" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="I11" s="61" t="s">
+      <c r="I11" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="61" t="s">
+      <c r="J11" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="63" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="16" thickTop="1">
-      <c r="A12" s="185"/>
-    </row>
-    <row r="13" spans="1:11" ht="16" thickBot="1">
-      <c r="A13" s="185"/>
-    </row>
-    <row r="14" spans="1:11" ht="16" thickTop="1">
-      <c r="A14" s="185"/>
-      <c r="C14" s="56" t="s">
+      <c r="M11">
+        <f>COUNTIF(F9:K11,"*")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" thickTop="1">
+      <c r="A12" s="183"/>
+      <c r="M12">
+        <f>COUNTIF(C4:G6,"*")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" thickBot="1">
+      <c r="A13" s="183"/>
+      <c r="M13">
+        <f>SUM(M10:M12)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16" thickTop="1">
+      <c r="A14" s="183"/>
+      <c r="C14" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="59" t="s">
+      <c r="H14" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="K14" s="64" t="s">
+      <c r="K14" s="62" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="185"/>
-      <c r="C15" s="63" t="s">
+    <row r="15" spans="1:13">
+      <c r="A15" s="183"/>
+      <c r="C15" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="60" t="s">
+      <c r="I15" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="K15" s="66" t="s">
+      <c r="K15" s="64" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" thickBot="1">
-      <c r="A16" s="185"/>
-      <c r="C16" s="57" t="s">
+    <row r="16" spans="1:13" ht="16" thickBot="1">
+      <c r="A16" s="183"/>
+      <c r="C16" s="55" t="s">
         <v>177</v>
       </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="61" t="s">
+      <c r="G16" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="H16" s="61" t="s">
+      <c r="H16" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="I16" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="J16" s="61" t="s">
+      <c r="J16" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="K16" s="65" t="s">
+      <c r="K16" s="63" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="185"/>
+      <c r="A17" s="183"/>
     </row>
     <row r="18" spans="1:11" ht="16" thickTop="1">
-      <c r="A18" s="185"/>
-      <c r="C18" s="56" t="s">
+      <c r="A18" s="183"/>
+      <c r="C18" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="67"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="65"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="186"/>
-      <c r="C19" s="63" t="s">
+      <c r="A19" s="184"/>
+      <c r="C19" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="68"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="66"/>
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1">
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="69"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="67"/>
     </row>
     <row r="21" spans="1:11" ht="16" thickTop="1"/>
     <row r="24" spans="1:11">
-      <c r="C24" s="187" t="s">
+      <c r="C24" s="185" t="s">
         <v>187</v>
       </c>
-      <c r="D24" s="188"/>
-      <c r="E24" s="188"/>
-      <c r="F24" s="188"/>
-      <c r="G24" s="188"/>
-      <c r="H24" s="188"/>
-      <c r="I24" s="188"/>
-      <c r="J24" s="188"/>
-      <c r="K24" s="189"/>
+      <c r="D24" s="186"/>
+      <c r="E24" s="186"/>
+      <c r="F24" s="186"/>
+      <c r="G24" s="186"/>
+      <c r="H24" s="186"/>
+      <c r="I24" s="186"/>
+      <c r="J24" s="186"/>
+      <c r="K24" s="187"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="C25" s="190"/>
-      <c r="D25" s="191"/>
-      <c r="E25" s="191"/>
-      <c r="F25" s="191"/>
-      <c r="G25" s="191"/>
-      <c r="H25" s="191"/>
-      <c r="I25" s="191"/>
-      <c r="J25" s="191"/>
-      <c r="K25" s="192"/>
+      <c r="C25" s="188"/>
+      <c r="D25" s="189"/>
+      <c r="E25" s="189"/>
+      <c r="F25" s="189"/>
+      <c r="G25" s="189"/>
+      <c r="H25" s="189"/>
+      <c r="I25" s="189"/>
+      <c r="J25" s="189"/>
+      <c r="K25" s="190"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="C27" s="187" t="s">
+      <c r="C27" s="185" t="s">
         <v>188</v>
       </c>
-      <c r="D27" s="188"/>
-      <c r="E27" s="188"/>
-      <c r="F27" s="188"/>
-      <c r="G27" s="188"/>
-      <c r="H27" s="188"/>
-      <c r="I27" s="188"/>
-      <c r="J27" s="188"/>
-      <c r="K27" s="189"/>
+      <c r="D27" s="186"/>
+      <c r="E27" s="186"/>
+      <c r="F27" s="186"/>
+      <c r="G27" s="186"/>
+      <c r="H27" s="186"/>
+      <c r="I27" s="186"/>
+      <c r="J27" s="186"/>
+      <c r="K27" s="187"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="C28" s="190"/>
-      <c r="D28" s="191"/>
-      <c r="E28" s="191"/>
-      <c r="F28" s="191"/>
-      <c r="G28" s="191"/>
-      <c r="H28" s="191"/>
-      <c r="I28" s="191"/>
-      <c r="J28" s="191"/>
-      <c r="K28" s="192"/>
+      <c r="C28" s="188"/>
+      <c r="D28" s="189"/>
+      <c r="E28" s="189"/>
+      <c r="F28" s="189"/>
+      <c r="G28" s="189"/>
+      <c r="H28" s="189"/>
+      <c r="I28" s="189"/>
+      <c r="J28" s="189"/>
+      <c r="K28" s="190"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11909,488 +11947,492 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="C1" s="200" t="s">
+    <row r="1" spans="1:14">
+      <c r="C1" s="198" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="202"/>
-    </row>
-    <row r="2" spans="1:11" ht="16" thickBot="1">
-      <c r="C2" s="203"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
-      <c r="I2" s="204"/>
-      <c r="J2" s="204"/>
-      <c r="K2" s="205"/>
-    </row>
-    <row r="3" spans="1:11" ht="16" thickBot="1"/>
-    <row r="4" spans="1:11">
-      <c r="C4" s="194" t="s">
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="200"/>
+    </row>
+    <row r="2" spans="1:14" ht="16" thickBot="1">
+      <c r="C2" s="201"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="203"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1"/>
+    <row r="4" spans="1:14">
+      <c r="C4" s="192" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="195"/>
-      <c r="E4" s="195"/>
-      <c r="F4" s="195"/>
-      <c r="G4" s="195"/>
-      <c r="H4" s="195"/>
-      <c r="I4" s="195"/>
-      <c r="J4" s="195"/>
-      <c r="K4" s="196"/>
-    </row>
-    <row r="5" spans="1:11" ht="16" thickBot="1">
-      <c r="C5" s="197"/>
-      <c r="D5" s="198"/>
-      <c r="E5" s="198"/>
-      <c r="F5" s="198"/>
-      <c r="G5" s="198"/>
-      <c r="H5" s="198"/>
-      <c r="I5" s="198"/>
-      <c r="J5" s="198"/>
-      <c r="K5" s="199"/>
-    </row>
-    <row r="7" spans="1:11" ht="16" thickBot="1"/>
-    <row r="8" spans="1:11" ht="16" thickTop="1">
-      <c r="A8" s="184" t="s">
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="I4" s="193"/>
+      <c r="J4" s="193"/>
+      <c r="K4" s="194"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="C5" s="195"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="196"/>
+      <c r="F5" s="196"/>
+      <c r="G5" s="196"/>
+      <c r="H5" s="196"/>
+      <c r="I5" s="196"/>
+      <c r="J5" s="196"/>
+      <c r="K5" s="197"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1"/>
+    <row r="8" spans="1:14" ht="16" thickTop="1">
+      <c r="A8" s="182" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59" t="s">
+      <c r="G8" s="57"/>
+      <c r="H8" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="50" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="185"/>
-      <c r="C9" s="62" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="183"/>
+      <c r="C9" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60" t="s">
+      <c r="F9" s="58"/>
+      <c r="G9" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="H9" s="60" t="s">
+      <c r="H9" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="K9" s="66" t="s">
+      <c r="K9" s="64" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" thickBot="1">
-      <c r="A10" s="185"/>
-      <c r="C10" s="54" t="s">
+    <row r="10" spans="1:14" ht="16" thickBot="1">
+      <c r="A10" s="183"/>
+      <c r="C10" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61" t="s">
+      <c r="F10" s="59"/>
+      <c r="G10" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="H10" s="61" t="s">
+      <c r="H10" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="I10" s="61" t="s">
+      <c r="I10" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="61" t="s">
+      <c r="J10" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="K10" s="55" t="s">
+      <c r="K10" s="53" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" thickTop="1">
-      <c r="A11" s="185"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-    </row>
-    <row r="12" spans="1:11" ht="16" thickBot="1">
-      <c r="A12" s="185"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-    </row>
-    <row r="13" spans="1:11" ht="16" thickTop="1">
-      <c r="A13" s="185"/>
-      <c r="C13" s="56" t="s">
+    <row r="11" spans="1:14" ht="16" thickTop="1">
+      <c r="A11" s="183"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="N11">
+        <f>COUNTIF(C8:K24,"*")</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16" thickBot="1">
+      <c r="A12" s="183"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickTop="1">
+      <c r="A13" s="183"/>
+      <c r="C13" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="J13" s="59" t="s">
+      <c r="J13" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="K13" s="52" t="s">
+      <c r="K13" s="50" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="185"/>
-      <c r="C14" s="63" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="183"/>
+      <c r="C14" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="58" t="s">
         <v>189</v>
       </c>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="60" t="s">
+      <c r="F14" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="G14" s="60" t="s">
+      <c r="G14" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="60" t="s">
+      <c r="H14" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="I14" s="60" t="s">
+      <c r="I14" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="J14" s="60" t="s">
+      <c r="J14" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="K14" s="66" t="s">
+      <c r="K14" s="64" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" thickBot="1">
-      <c r="A15" s="185"/>
-      <c r="C15" s="57" t="s">
+    <row r="15" spans="1:14" ht="16" thickBot="1">
+      <c r="A15" s="183"/>
+      <c r="C15" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="59" t="s">
         <v>195</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61" t="s">
+      <c r="H15" s="59"/>
+      <c r="I15" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="J15" s="61" t="s">
+      <c r="J15" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="K15" s="55" t="s">
+      <c r="K15" s="53" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" thickTop="1">
-      <c r="A16" s="185"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
+    <row r="16" spans="1:14" ht="16" thickTop="1">
+      <c r="A16" s="183"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
     </row>
     <row r="17" spans="1:11" ht="16" thickBot="1">
-      <c r="A17" s="185"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
+      <c r="A17" s="183"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
     </row>
     <row r="18" spans="1:11" ht="16" thickTop="1">
-      <c r="A18" s="185"/>
-      <c r="C18" s="56" t="s">
+      <c r="A18" s="183"/>
+      <c r="C18" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="F18" s="59" t="s">
+      <c r="F18" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G18" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="H18" s="59" t="s">
+      <c r="H18" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="I18" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="J18" s="59"/>
-      <c r="K18" s="52" t="s">
+      <c r="J18" s="57"/>
+      <c r="K18" s="50" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="185"/>
-      <c r="C19" s="63" t="s">
+      <c r="A19" s="183"/>
+      <c r="C19" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="H19" s="60" t="s">
+      <c r="H19" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="I19" s="60" t="s">
+      <c r="I19" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="J19" s="60" t="s">
+      <c r="J19" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="K19" s="66" t="s">
+      <c r="K19" s="64" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1">
-      <c r="A20" s="185"/>
-      <c r="C20" s="57" t="s">
+      <c r="A20" s="183"/>
+      <c r="C20" s="55" t="s">
         <v>197</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="H20" s="61" t="s">
+      <c r="H20" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="61" t="s">
+      <c r="I20" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="J20" s="61"/>
-      <c r="K20" s="55"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="53"/>
     </row>
     <row r="21" spans="1:11" ht="17" thickTop="1" thickBot="1">
-      <c r="A21" s="185"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
+      <c r="A21" s="183"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78"/>
     </row>
     <row r="22" spans="1:11" ht="16" thickTop="1">
-      <c r="A22" s="185"/>
-      <c r="C22" s="56" t="s">
+      <c r="A22" s="183"/>
+      <c r="C22" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59" t="s">
+      <c r="E22" s="57"/>
+      <c r="F22" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="G22" s="59" t="s">
+      <c r="G22" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H22" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="I22" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="K22" s="81"/>
+      <c r="K22" s="79"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="185"/>
-      <c r="C23" s="63" t="s">
+      <c r="A23" s="183"/>
+      <c r="C23" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="H23" s="60" t="s">
+      <c r="H23" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="I23" s="60" t="s">
+      <c r="I23" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="J23" s="60" t="s">
+      <c r="J23" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="K23" s="68" t="s">
+      <c r="K23" s="66" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" thickBot="1">
-      <c r="A24" s="186"/>
-      <c r="C24" s="57" t="s">
+      <c r="A24" s="184"/>
+      <c r="C24" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61" t="s">
+      <c r="E24" s="59"/>
+      <c r="F24" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="61" t="s">
+      <c r="G24" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="H24" s="61" t="s">
+      <c r="H24" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="I24" s="61" t="s">
+      <c r="I24" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="J24" s="61" t="s">
+      <c r="J24" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="K24" s="82"/>
+      <c r="K24" s="80"/>
     </row>
     <row r="25" spans="1:11" ht="16" thickTop="1"/>
     <row r="27" spans="1:11">
-      <c r="C27" s="187" t="s">
+      <c r="C27" s="185" t="s">
         <v>188</v>
       </c>
-      <c r="D27" s="188"/>
-      <c r="E27" s="188"/>
-      <c r="F27" s="188"/>
-      <c r="G27" s="188"/>
-      <c r="H27" s="188"/>
-      <c r="I27" s="188"/>
-      <c r="J27" s="188"/>
-      <c r="K27" s="189"/>
+      <c r="D27" s="186"/>
+      <c r="E27" s="186"/>
+      <c r="F27" s="186"/>
+      <c r="G27" s="186"/>
+      <c r="H27" s="186"/>
+      <c r="I27" s="186"/>
+      <c r="J27" s="186"/>
+      <c r="K27" s="187"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="C28" s="190"/>
-      <c r="D28" s="191"/>
-      <c r="E28" s="191"/>
-      <c r="F28" s="191"/>
-      <c r="G28" s="191"/>
-      <c r="H28" s="191"/>
-      <c r="I28" s="191"/>
-      <c r="J28" s="191"/>
-      <c r="K28" s="192"/>
+      <c r="C28" s="188"/>
+      <c r="D28" s="189"/>
+      <c r="E28" s="189"/>
+      <c r="F28" s="189"/>
+      <c r="G28" s="189"/>
+      <c r="H28" s="189"/>
+      <c r="I28" s="189"/>
+      <c r="J28" s="189"/>
+      <c r="K28" s="190"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -12421,211 +12463,211 @@
   <sheetData>
     <row r="2" spans="2:10" ht="16" thickBot="1"/>
     <row r="3" spans="2:10" ht="16" thickTop="1">
-      <c r="B3" s="50"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="52"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="62"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="66"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="2:10" ht="16" thickBot="1">
-      <c r="B5" s="54"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="55"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="2:10" ht="16" thickTop="1">
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
     </row>
     <row r="7" spans="2:10" ht="16" thickBot="1">
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
     </row>
     <row r="8" spans="2:10" ht="16" thickTop="1">
-      <c r="B8" s="56"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="52"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="50"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="63"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="66"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="64"/>
     </row>
     <row r="10" spans="2:10" ht="16" thickBot="1">
-      <c r="B10" s="57"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="55"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="2:10" ht="16" thickTop="1">
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
     </row>
     <row r="12" spans="2:10" ht="16" thickBot="1">
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
     </row>
     <row r="13" spans="2:10" ht="16" thickTop="1">
-      <c r="B13" s="56"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="52"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="50"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="63"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="66"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="64"/>
     </row>
     <row r="15" spans="2:10" ht="16" thickBot="1">
-      <c r="B15" s="57"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="55"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="53"/>
     </row>
     <row r="16" spans="2:10" ht="17" thickTop="1" thickBot="1">
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
     </row>
     <row r="17" spans="2:10" ht="16" thickTop="1">
-      <c r="B17" s="56"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="81"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="79"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="63"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="68"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="66"/>
     </row>
     <row r="19" spans="2:10" ht="16" thickBot="1">
-      <c r="B19" s="57"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="82"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="80"/>
     </row>
     <row r="20" spans="2:10" ht="16" thickTop="1">
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12639,52 +12681,52 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N15"/>
+  <dimension ref="B1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="2:14" ht="35" customHeight="1">
-      <c r="D1" s="212" t="s">
+    <row r="1" spans="2:19" ht="35" customHeight="1">
+      <c r="D1" s="210" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="214"/>
-    </row>
-    <row r="2" spans="2:14" ht="35" customHeight="1" thickBot="1"/>
-    <row r="3" spans="2:14" ht="35" customHeight="1">
-      <c r="B3" s="206" t="s">
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="212"/>
+    </row>
+    <row r="2" spans="2:19" ht="35" customHeight="1" thickBot="1"/>
+    <row r="3" spans="2:19" ht="35" customHeight="1">
+      <c r="B3" s="204" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="207"/>
-      <c r="E3" s="70" t="s">
+      <c r="C3" s="205"/>
+      <c r="E3" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="I3" s="73"/>
-    </row>
-    <row r="4" spans="2:14" ht="35" customHeight="1">
-      <c r="B4" s="208"/>
-      <c r="C4" s="209"/>
-      <c r="E4" s="74" t="s">
+      <c r="I3" s="71"/>
+    </row>
+    <row r="4" spans="2:19" ht="35" customHeight="1">
+      <c r="B4" s="206"/>
+      <c r="C4" s="207"/>
+      <c r="E4" s="72" t="s">
         <v>198</v>
       </c>
       <c r="F4" s="12" t="s">
@@ -12696,115 +12738,119 @@
       <c r="H4" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="I4" s="86" t="s">
+      <c r="I4" s="84" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="35" customHeight="1" thickBot="1">
-      <c r="B5" s="208"/>
-      <c r="C5" s="209"/>
-      <c r="E5" s="95"/>
+    <row r="5" spans="2:19" ht="35" customHeight="1" thickBot="1">
+      <c r="B5" s="206"/>
+      <c r="C5" s="207"/>
+      <c r="E5" s="93"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="94" t="s">
         <v>189</v>
       </c>
-      <c r="H5" s="96" t="s">
+      <c r="H5" s="94" t="s">
         <v>189</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="95" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="35" customHeight="1">
-      <c r="B6" s="208"/>
-      <c r="C6" s="209"/>
-      <c r="E6" s="118" t="s">
+      <c r="S5">
+        <f>COUNTIF(E3:N15,"*")</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="35" customHeight="1">
+      <c r="B6" s="206"/>
+      <c r="C6" s="207"/>
+      <c r="E6" s="116" t="s">
         <v>208</v>
       </c>
-      <c r="F6" s="119" t="s">
+      <c r="F6" s="117" t="s">
         <v>200</v>
       </c>
-      <c r="G6" s="120" t="s">
+      <c r="G6" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="H6" s="119" t="s">
+      <c r="H6" s="117" t="s">
         <v>192</v>
       </c>
-      <c r="I6" s="121" t="s">
+      <c r="I6" s="119" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="35" customHeight="1">
-      <c r="B7" s="208"/>
-      <c r="C7" s="209"/>
-      <c r="E7" s="122" t="s">
+    <row r="7" spans="2:19" ht="35" customHeight="1">
+      <c r="B7" s="206"/>
+      <c r="C7" s="207"/>
+      <c r="E7" s="120" t="s">
         <v>200</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="G7" s="123" t="s">
+      <c r="G7" s="121" t="s">
         <v>192</v>
       </c>
-      <c r="H7" s="124" t="s">
+      <c r="H7" s="122" t="s">
         <v>202</v>
       </c>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="84" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="35" customHeight="1" thickBot="1">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="E8" s="76" t="s">
+    <row r="8" spans="2:19" ht="35" customHeight="1" thickBot="1">
+      <c r="B8" s="208"/>
+      <c r="C8" s="209"/>
+      <c r="E8" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="76" t="s">
         <v>193</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="I8" s="79"/>
-    </row>
-    <row r="9" spans="2:14" ht="35" customHeight="1" thickBot="1"/>
-    <row r="10" spans="2:14" ht="35" customHeight="1">
-      <c r="B10" s="206" t="s">
+      <c r="I8" s="77"/>
+    </row>
+    <row r="9" spans="2:19" ht="35" customHeight="1" thickBot="1"/>
+    <row r="10" spans="2:19" ht="35" customHeight="1">
+      <c r="B10" s="204" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="207"/>
-      <c r="E10" s="70" t="s">
+      <c r="C10" s="205"/>
+      <c r="E10" s="68" t="s">
         <v>177</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="69" t="s">
         <v>177</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="109" t="s">
+      <c r="G10" s="70"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="K10" s="71" t="s">
+      <c r="K10" s="69" t="s">
         <v>179</v>
       </c>
-      <c r="L10" s="110" t="s">
+      <c r="L10" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="M10" s="71" t="s">
+      <c r="M10" s="69" t="s">
         <v>174</v>
       </c>
-      <c r="N10" s="111" t="s">
+      <c r="N10" s="109" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="35" customHeight="1">
-      <c r="B11" s="208"/>
-      <c r="C11" s="209"/>
-      <c r="E11" s="74" t="s">
+    <row r="11" spans="2:19" ht="35" customHeight="1">
+      <c r="B11" s="206"/>
+      <c r="C11" s="207"/>
+      <c r="E11" s="72" t="s">
         <v>178</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -12817,121 +12863,121 @@
       <c r="I11" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J11" s="112"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="113"/>
-      <c r="M11" s="113"/>
-      <c r="N11" s="75"/>
-    </row>
-    <row r="12" spans="2:14" ht="35" customHeight="1" thickBot="1">
-      <c r="B12" s="208"/>
-      <c r="C12" s="209"/>
-      <c r="E12" s="95" t="s">
+      <c r="J11" s="110"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="73"/>
+    </row>
+    <row r="12" spans="2:19" ht="35" customHeight="1" thickBot="1">
+      <c r="B12" s="206"/>
+      <c r="C12" s="207"/>
+      <c r="E12" s="93" t="s">
         <v>178</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G12" s="96" t="s">
+      <c r="G12" s="94" t="s">
         <v>209</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="114" t="s">
+      <c r="I12" s="104"/>
+      <c r="J12" s="112" t="s">
         <v>179</v>
       </c>
-      <c r="K12" s="115" t="s">
+      <c r="K12" s="113" t="s">
         <v>174</v>
       </c>
-      <c r="L12" s="116" t="s">
+      <c r="L12" s="114" t="s">
         <v>174</v>
       </c>
-      <c r="M12" s="115"/>
-      <c r="N12" s="117" t="s">
+      <c r="M12" s="113"/>
+      <c r="N12" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="35" customHeight="1">
-      <c r="B13" s="208"/>
-      <c r="C13" s="209"/>
-      <c r="E13" s="99" t="s">
+    <row r="13" spans="2:19" ht="35" customHeight="1">
+      <c r="B13" s="206"/>
+      <c r="C13" s="207"/>
+      <c r="E13" s="97" t="s">
         <v>184</v>
       </c>
-      <c r="F13" s="100"/>
-      <c r="G13" s="101" t="s">
+      <c r="F13" s="98"/>
+      <c r="G13" s="99" t="s">
         <v>210</v>
       </c>
-      <c r="H13" s="100" t="s">
+      <c r="H13" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="I13" s="102" t="s">
+      <c r="I13" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="J13" s="84" t="s">
+      <c r="J13" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="K13" s="88"/>
-      <c r="L13" s="107" t="s">
+      <c r="K13" s="86"/>
+      <c r="L13" s="105" t="s">
         <v>173</v>
       </c>
-      <c r="M13" s="88"/>
-      <c r="N13" s="108" t="s">
+      <c r="M13" s="86"/>
+      <c r="N13" s="106" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="35" customHeight="1">
-      <c r="B14" s="208"/>
-      <c r="C14" s="209"/>
-      <c r="E14" s="87" t="s">
+    <row r="14" spans="2:19" ht="35" customHeight="1">
+      <c r="B14" s="206"/>
+      <c r="C14" s="207"/>
+      <c r="E14" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="83" t="s">
+      <c r="F14" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="G14" s="84"/>
-      <c r="H14" s="85" t="s">
+      <c r="G14" s="82"/>
+      <c r="H14" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="I14" s="103" t="s">
+      <c r="I14" s="101" t="s">
         <v>210</v>
       </c>
-      <c r="J14" s="88" t="s">
+      <c r="J14" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="K14" s="83"/>
-      <c r="L14" s="84" t="s">
+      <c r="K14" s="81"/>
+      <c r="L14" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="M14" s="85"/>
-      <c r="N14" s="89" t="s">
+      <c r="M14" s="83"/>
+      <c r="N14" s="87" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="35" customHeight="1" thickBot="1">
-      <c r="B15" s="210"/>
-      <c r="C15" s="211"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91" t="s">
+    <row r="15" spans="2:19" ht="35" customHeight="1" thickBot="1">
+      <c r="B15" s="208"/>
+      <c r="C15" s="209"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="89" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="92" t="s">
+      <c r="G15" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="H15" s="91" t="s">
+      <c r="H15" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="104" t="s">
+      <c r="I15" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="91" t="s">
         <v>175</v>
       </c>
-      <c r="K15" s="91"/>
-      <c r="L15" s="92" t="s">
+      <c r="K15" s="89"/>
+      <c r="L15" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="M15" s="91"/>
-      <c r="N15" s="94" t="s">
+      <c r="M15" s="89"/>
+      <c r="N15" s="92" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>